<commit_message>
Added A small HowTo, OutlookScraper and JIRAIssueCreator
</commit_message>
<xml_diff>
--- a/Mappingtable.xlsx
+++ b/Mappingtable.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51B5D8BE-0B7D-4D68-8C6D-B814819DC7F0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>JIRAURL</t>
   </si>
@@ -37,31 +36,34 @@
     <t>Label</t>
   </si>
   <si>
-    <t>jira.example.com</t>
-  </si>
-  <si>
-    <t>test</t>
+    <t>Example</t>
+  </si>
+  <si>
+    <t>ProjectID</t>
+  </si>
+  <si>
+    <t>IssueType</t>
+  </si>
+  <si>
+    <t>Task</t>
+  </si>
+  <si>
+    <t>http://jira.example.com</t>
+  </si>
+  <si>
+    <t>Test</t>
   </si>
   <si>
     <t>test123</t>
   </si>
   <si>
     <t>test@test.at</t>
-  </si>
-  <si>
-    <t>Example</t>
-  </si>
-  <si>
-    <t>jira2.example.com</t>
-  </si>
-  <si>
-    <t>Example2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -383,20 +385,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -407,50 +409,45 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2">
+        <v>10000</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
         <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{05DCF4B7-0421-4ACA-9150-30F9CEAE931E}"/>
-    <hyperlink ref="D3" r:id="rId2" xr:uid="{FD0A1CFE-0041-418B-9F8C-A4CFF27AC464}"/>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="F2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Changed Mappingtable from projectId to projectKey
</commit_message>
<xml_diff>
--- a/Mappingtable.xlsx
+++ b/Mappingtable.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>JIRAURL</t>
   </si>
@@ -39,22 +39,25 @@
     <t>Example</t>
   </si>
   <si>
-    <t>ProjectID</t>
-  </si>
-  <si>
     <t>IssueType</t>
   </si>
   <si>
     <t>Task</t>
   </si>
   <si>
+    <t>ProjectKey</t>
+  </si>
+  <si>
     <t>http://jira.example.com</t>
   </si>
   <si>
-    <t>Test</t>
+    <t>test</t>
   </si>
   <si>
     <t>test123</t>
+  </si>
+  <si>
+    <t>TST</t>
   </si>
   <si>
     <t>test@test.at</t>
@@ -389,13 +392,14 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -409,10 +413,10 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
         <v>6</v>
-      </c>
-      <c r="E1" t="s">
-        <v>7</v>
       </c>
       <c r="F1" t="s">
         <v>3</v>
@@ -431,14 +435,14 @@
       <c r="C2" t="s">
         <v>11</v>
       </c>
-      <c r="D2">
-        <v>10000</v>
+      <c r="D2" t="s">
+        <v>12</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G2" t="s">
         <v>5</v>

</xml_diff>